<commit_message>
ajout de gitignore et suppression de fichiers inutiles
</commit_message>
<xml_diff>
--- a/Liste.xlsx
+++ b/Liste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsoucy/GitHub/PDFExamens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE53B08-3523-DE45-A997-BC7A55736792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F02273-87A2-E84D-A9A1-BF2D9711062C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11920" yWindow="5980" windowWidth="27760" windowHeight="16680" xr2:uid="{FB1C3549-BE42-1643-B0F7-08881D6C1D29}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Prénom et nom</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Local</t>
   </si>
   <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
     <t>Ismael Jankelevich III</t>
   </si>
   <si>
@@ -87,6 +78,18 @@
   </si>
   <si>
     <t>Yramasse Delaroche</t>
+  </si>
+  <si>
+    <t>NRC</t>
+  </si>
+  <si>
+    <t>J. Soucy</t>
+  </si>
+  <si>
+    <t>Enseignant</t>
+  </si>
+  <si>
+    <t>M. Genest</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCD2B96-4E88-4E45-BF13-E39F352F0E77}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -470,7 +473,7 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,10 +487,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -500,13 +506,16 @@
       <c r="D2">
         <v>2880</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>12345</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>121212121</v>
@@ -518,13 +527,16 @@
       <c r="D3">
         <v>2880</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>12345</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
       </c>
       <c r="B4">
         <v>987654321</v>
@@ -536,13 +548,16 @@
       <c r="D4">
         <v>2880</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>12345</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>787654321</v>
@@ -554,13 +569,16 @@
       <c r="D5">
         <v>1112</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>12345</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>333444555</v>
@@ -572,13 +590,16 @@
       <c r="D6">
         <v>1112</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>12345</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>121212121</v>
@@ -590,13 +611,16 @@
       <c r="D7">
         <v>1112</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>54321</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>987654321</v>
@@ -608,13 +632,16 @@
       <c r="D8">
         <v>1112</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>54321</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>787654321</v>
@@ -626,13 +653,16 @@
       <c r="D9">
         <v>1112</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>54321</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>787654321</v>
@@ -644,13 +674,16 @@
       <c r="D10">
         <v>1112</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>54321</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>787654321</v>
@@ -662,8 +695,11 @@
       <c r="D11">
         <v>1112</v>
       </c>
-      <c r="E11" t="s">
-        <v>7</v>
+      <c r="E11">
+        <v>54321</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>